<commit_message>
more requirements classified and first approach for ensemble classifier
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/evaluation_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,76 +562,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4692631578947368</v>
+        <v>0.5154639175257731</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5748394568513311</v>
+        <v>0.5501022163793501</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5351168948011054</v>
+        <v>0.5262617327632807</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4593856714900366</v>
+        <v>0.4807650635718315</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5986315789473684</v>
+        <v>0.5670103092783505</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6790208888014515</v>
+        <v>0.632590446989868</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6003582032003085</v>
+        <v>0.5729038281979457</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5832605072305095</v>
+        <v>0.5441641680825956</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5987719298245613</v>
+        <v>0.5670103092783505</v>
       </c>
       <c r="K2" t="n">
-        <v>0.689521125732907</v>
+        <v>0.6212897563171373</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5968126727074095</v>
+        <v>0.5693567251461988</v>
       </c>
       <c r="M2" t="n">
-        <v>0.5861015741695719</v>
+        <v>0.5577232950839509</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6540350877192982</v>
+        <v>0.6082474226804123</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6704026913918556</v>
+        <v>0.6126692698575859</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6645396825396827</v>
+        <v>0.6113813946631284</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.6457168333153067</v>
+        <v>0.5999856053719078</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5328421052631579</v>
+        <v>0.468041237113402</v>
       </c>
       <c r="S2" t="n">
-        <v>0.5637680760720221</v>
+        <v>0.5370471273372495</v>
       </c>
       <c r="T2" t="n">
-        <v>0.4656121071910546</v>
+        <v>0.468391567153177</v>
       </c>
       <c r="U2" t="n">
-        <v>0.443899050416654</v>
+        <v>0.4608091376274689</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5328421052631579</v>
+        <v>0.468041237113402</v>
       </c>
       <c r="W2" t="n">
-        <v>0.5637680760720221</v>
+        <v>0.5370471273372495</v>
       </c>
       <c r="X2" t="n">
-        <v>0.4656121071910546</v>
+        <v>0.468391567153177</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.443899050416654</v>
+        <v>0.4608091376274689</v>
       </c>
     </row>
     <row r="3">
@@ -641,76 +641,76 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.720280701754386</v>
+        <v>0.6948453608247424</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7421726703771394</v>
+        <v>0.7238971077299784</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7289464687359424</v>
+        <v>0.6940940586761021</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7181376372258421</v>
+        <v>0.6912806583050726</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7096140350877193</v>
+        <v>0.7092783505154638</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7272525859555581</v>
+        <v>0.7373028001315965</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7146724503566608</v>
+        <v>0.707936507936508</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7021189830609795</v>
+        <v>0.7084164375674769</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7096140350877193</v>
+        <v>0.7092783505154638</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7272525859555581</v>
+        <v>0.7373028001315965</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7146724503566608</v>
+        <v>0.707936507936508</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7021189830609795</v>
+        <v>0.7084164375674769</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7384912280701755</v>
+        <v>0.6927835051546392</v>
       </c>
       <c r="O3" t="n">
-        <v>0.7576135988194812</v>
+        <v>0.7163858237984029</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7176657027183342</v>
+        <v>0.6918688879060396</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.7188338995054593</v>
+        <v>0.6877167398491423</v>
       </c>
       <c r="R3" t="n">
-        <v>0.7517192982456141</v>
+        <v>0.7319587628865979</v>
       </c>
       <c r="S3" t="n">
-        <v>0.7898804097862923</v>
+        <v>0.7563400033527428</v>
       </c>
       <c r="T3" t="n">
-        <v>0.7238586209112526</v>
+        <v>0.7302452208953758</v>
       </c>
       <c r="U3" t="n">
-        <v>0.7301709473752359</v>
+        <v>0.726973369957835</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7517192982456141</v>
+        <v>0.7319587628865979</v>
       </c>
       <c r="W3" t="n">
-        <v>0.7898804097862923</v>
+        <v>0.7563400033527428</v>
       </c>
       <c r="X3" t="n">
-        <v>0.7238586209112526</v>
+        <v>0.7302452208953758</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.7301709473752359</v>
+        <v>0.726973369957835</v>
       </c>
     </row>
     <row r="4">
@@ -720,76 +720,76 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7491929824561404</v>
+        <v>0.6907216494845361</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7758857112481153</v>
+        <v>0.7115741915905511</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7362070561017928</v>
+        <v>0.6895660720428524</v>
       </c>
       <c r="E4" t="n">
-        <v>0.732392851248574</v>
+        <v>0.6864554750414388</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7571228070175439</v>
+        <v>0.7278350515463917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7818726241079181</v>
+        <v>0.7531931742185816</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7454885932780668</v>
+        <v>0.7258115877930119</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7429673824479615</v>
+        <v>0.7283094043839362</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7571228070175439</v>
+        <v>0.7278350515463917</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7818726241079181</v>
+        <v>0.7531931742185816</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7454885932780668</v>
+        <v>0.7258115877930119</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7429673824479615</v>
+        <v>0.7283094043839362</v>
       </c>
       <c r="N4" t="n">
-        <v>0.7254736842105263</v>
+        <v>0.7010309278350516</v>
       </c>
       <c r="O4" t="n">
-        <v>0.7840765034437743</v>
+        <v>0.7242188254153156</v>
       </c>
       <c r="P4" t="n">
-        <v>0.6797299659404923</v>
+        <v>0.697544842498403</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.6854345908910837</v>
+        <v>0.6938546586702822</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7333684210526317</v>
+        <v>0.7298969072164948</v>
       </c>
       <c r="S4" t="n">
-        <v>0.7592166164878328</v>
+        <v>0.7576090174642015</v>
       </c>
       <c r="T4" t="n">
-        <v>0.6856957779063043</v>
+        <v>0.726889773453241</v>
       </c>
       <c r="U4" t="n">
-        <v>0.6868593160963729</v>
+        <v>0.7267085276261819</v>
       </c>
       <c r="V4" t="n">
-        <v>0.7333684210526317</v>
+        <v>0.7298969072164948</v>
       </c>
       <c r="W4" t="n">
-        <v>0.7592166164878328</v>
+        <v>0.7576090174642015</v>
       </c>
       <c r="X4" t="n">
-        <v>0.6856957779063043</v>
+        <v>0.726889773453241</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.6868593160963729</v>
+        <v>0.7267085276261819</v>
       </c>
     </row>
     <row r="5">
@@ -799,28 +799,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7173684210526317</v>
+        <v>0.6556701030927835</v>
       </c>
       <c r="C5" t="n">
-        <v>0.72304726194671</v>
+        <v>0.6688792251107503</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6874200886832466</v>
+        <v>0.652435991940636</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6804903319394386</v>
+        <v>0.6441128945624456</v>
       </c>
       <c r="F5" t="n">
-        <v>0.746421052631579</v>
+        <v>0.7278350515463917</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7916595541992182</v>
+        <v>0.7435934855381079</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7300466550992867</v>
+        <v>0.7235824856258292</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7283730453617357</v>
+        <v>0.7217225062629988</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -835,28 +835,28 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6752280701754387</v>
+        <v>0.6536082474226804</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6148787699897378</v>
+        <v>0.6855695759289765</v>
       </c>
       <c r="P5" t="n">
-        <v>0.6052186877450035</v>
+        <v>0.6482008943928449</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.5780750244846103</v>
+        <v>0.6359419755845588</v>
       </c>
       <c r="R5" t="n">
-        <v>0.7016842105263159</v>
+        <v>0.6989690721649485</v>
       </c>
       <c r="S5" t="n">
-        <v>0.691889132252842</v>
+        <v>0.7414403171431545</v>
       </c>
       <c r="T5" t="n">
-        <v>0.6311000578368999</v>
+        <v>0.6954818418595508</v>
       </c>
       <c r="U5" t="n">
-        <v>0.6071340708584987</v>
+        <v>0.6920731469137873</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
@@ -869,6 +869,85 @@
       </c>
       <c r="Y5" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.6927835051546392</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7148699056859644</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.6954189395056268</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6884880347501156</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7278350515463917</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.7645850209996984</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.7285566858322277</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7282455651959145</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.7154639175257731</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.7468185316526796</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.7154906875030714</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.7133057519877879</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.6969072164948453</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.7118356590354301</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.6967310432945107</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.6927819415178955</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.7443298969072166</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.7666078794697349</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.7428876111848248</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.742514809634382</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.7154639175257731</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.7468185316526796</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.7154906875030714</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.7133057519877879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more detailed evaluation for SVM classification with PCA
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/evaluation_metrics.xlsx
@@ -565,73 +565,73 @@
         <v>0.6264699153511782</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6827159843522745</v>
+        <v>0.6881615054955936</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6341363949088408</v>
+        <v>0.6264699153511782</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6232816386862253</v>
+        <v>0.6221844651985571</v>
       </c>
       <c r="F2" t="n">
         <v>0.6865248226950355</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7287601146484344</v>
+        <v>0.7351167062838367</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6936234458695759</v>
+        <v>0.6865248226950355</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6845269694085717</v>
+        <v>0.6844945096892918</v>
       </c>
       <c r="J2" t="n">
         <v>0.6844200411805079</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7107004035036072</v>
+        <v>0.7148942439039832</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6905591429554278</v>
+        <v>0.6844200411805079</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6849952631923424</v>
+        <v>0.6839613283381253</v>
       </c>
       <c r="N2" t="n">
         <v>0.7789750629146649</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7887438470430125</v>
+        <v>0.7926823995174128</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7819258440218192</v>
+        <v>0.7789750629146649</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.7786414582326626</v>
+        <v>0.7790072107894227</v>
       </c>
       <c r="R2" t="n">
         <v>0.7126058110272249</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7653777173604875</v>
+        <v>0.7708159889374424</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7160913804118139</v>
+        <v>0.7126058110272249</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7144583453858951</v>
+        <v>0.715969873474698</v>
       </c>
       <c r="V2" t="n">
         <v>0.7147334706016929</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7677645034703857</v>
+        <v>0.7730195373019669</v>
       </c>
       <c r="X2" t="n">
-        <v>0.7182647550248168</v>
+        <v>0.7147334706016929</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.7198769327254908</v>
+        <v>0.7213536650873087</v>
       </c>
     </row>
     <row r="3">
@@ -644,73 +644,73 @@
         <v>0.7875543353923588</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7961054743554408</v>
+        <v>0.7985956243374288</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7904938326207677</v>
+        <v>0.7875543353923588</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7874989211781334</v>
+        <v>0.7873394143488996</v>
       </c>
       <c r="F3" t="n">
         <v>0.8004118050789293</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8094222284572936</v>
+        <v>0.8128679272287336</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8021935721657083</v>
+        <v>0.8004118050789293</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8008522647585214</v>
+        <v>0.801663318551846</v>
       </c>
       <c r="J3" t="n">
         <v>0.8133150308853809</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8195430049975749</v>
+        <v>0.8219350976610016</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8127075040542533</v>
+        <v>0.8133150308853809</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8135166729510624</v>
+        <v>0.8150161887268537</v>
       </c>
       <c r="N3" t="n">
         <v>0.8305193319606496</v>
       </c>
       <c r="O3" t="n">
-        <v>0.837193075429379</v>
+        <v>0.8391740644712609</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8327912428129146</v>
+        <v>0.8305193319606496</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8303197603269638</v>
+        <v>0.8300626228518213</v>
       </c>
       <c r="R3" t="n">
         <v>0.8519103180050331</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8581773594258451</v>
+        <v>0.8595560068448369</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8540906678460859</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="U3" t="n">
-        <v>0.851657662052042</v>
+        <v>0.8510766315601531</v>
       </c>
       <c r="V3" t="n">
         <v>0.8561885152139099</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8648990865911582</v>
+        <v>0.8657432086529147</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8576424885743773</v>
+        <v>0.8561885152139099</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.8563287769495626</v>
+        <v>0.8559497519229347</v>
       </c>
     </row>
     <row r="4">
@@ -723,73 +723,73 @@
         <v>0.8153283001601463</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8203512010864952</v>
+        <v>0.8231285042630135</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8180544007076515</v>
+        <v>0.8153283001601463</v>
       </c>
       <c r="E4" t="n">
-        <v>0.81454300740871</v>
+        <v>0.8145030727138709</v>
       </c>
       <c r="F4" t="n">
         <v>0.8540150995195608</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8584375271084786</v>
+        <v>0.8611739633378448</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8558166740380363</v>
+        <v>0.8540150995195608</v>
       </c>
       <c r="I4" t="n">
-        <v>0.853765038304458</v>
+        <v>0.854172320614113</v>
       </c>
       <c r="J4" t="n">
         <v>0.8325326012354154</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8379911588239762</v>
+        <v>0.8398044924418351</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8347532065457763</v>
+        <v>0.8325326012354154</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8324683386775058</v>
+        <v>0.8322725549148501</v>
       </c>
       <c r="N4" t="n">
         <v>0.8347517730496454</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8377286010305932</v>
+        <v>0.838719606885767</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8349467049977886</v>
+        <v>0.8347517730496454</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8336138906781352</v>
+        <v>0.8340428381639159</v>
       </c>
       <c r="R4" t="n">
         <v>0.8476549988560971</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8511095726412055</v>
+        <v>0.8524934376831117</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8469195783576587</v>
+        <v>0.8476549988560971</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8459091711891444</v>
+        <v>0.8469769510436667</v>
       </c>
       <c r="V4" t="n">
         <v>0.8498055364905056</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8533434907698604</v>
+        <v>0.8545729195418804</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8489195783576587</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8480058464437145</v>
+        <v>0.8490848129987272</v>
       </c>
     </row>
     <row r="5">
@@ -802,25 +802,25 @@
         <v>0.8047357584076871</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8142600841255033</v>
+        <v>0.8147226913677754</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8035751142562289</v>
+        <v>0.8047357584076871</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8016592175761478</v>
+        <v>0.8026002501243894</v>
       </c>
       <c r="F5" t="n">
         <v>0.8390528483184626</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8470024280844715</v>
+        <v>0.8478250140868472</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8391191950464396</v>
+        <v>0.8390528483184626</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8384401787609119</v>
+        <v>0.8388895481124227</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -838,25 +838,25 @@
         <v>0.8197208876687258</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8339583987003557</v>
+        <v>0.832594934784729</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8185533687159074</v>
+        <v>0.8197208876687258</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.8171909290261203</v>
+        <v>0.8173006130378528</v>
       </c>
       <c r="R5" t="n">
         <v>0.8455044612216884</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8574598263345067</v>
+        <v>0.8567157216617579</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8445858027421493</v>
+        <v>0.8455044612216884</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8446122300021788</v>
+        <v>0.8447762295277957</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
@@ -881,73 +881,73 @@
         <v>0.6844886753603293</v>
       </c>
       <c r="C6" t="n">
-        <v>0.714889690513193</v>
+        <v>0.718150479358624</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6900889724310776</v>
+        <v>0.6844886753603293</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6809764049062169</v>
+        <v>0.678974110704153</v>
       </c>
       <c r="F6" t="n">
         <v>0.7059254175245938</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7476393139269615</v>
+        <v>0.7488661302646362</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7086834733893557</v>
+        <v>0.7059254175245938</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7051306310363861</v>
+        <v>0.7033312625658155</v>
       </c>
       <c r="J6" t="n">
         <v>0.7037977579501258</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7504883570820404</v>
+        <v>0.7520611880317394</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7062523956951201</v>
+        <v>0.7037977579501258</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7011090936252452</v>
+        <v>0.6995047456688194</v>
       </c>
       <c r="N6" t="n">
         <v>0.7145504461221688</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7379579541231716</v>
+        <v>0.7359756673928738</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7167933067964027</v>
+        <v>0.7145504461221688</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.7099926459433896</v>
+        <v>0.7078176161253705</v>
       </c>
       <c r="R6" t="n">
         <v>0.7188515213909861</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7469568346476814</v>
+        <v>0.7455727442185192</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7204403656199321</v>
+        <v>0.7188515213909861</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7143542121924914</v>
+        <v>0.712972901679728</v>
       </c>
       <c r="V6" t="n">
         <v>0.7037977579501258</v>
       </c>
       <c r="W6" t="n">
-        <v>0.7504883570820404</v>
+        <v>0.7520611880317394</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7062523956951201</v>
+        <v>0.7037977579501258</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.7011090936252452</v>
+        <v>0.6995047456688194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved ensemble model by adding accuracies of individual classifiers as weights
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/evaluation_metrics.xlsx
@@ -878,76 +878,76 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6844886753603293</v>
+        <v>0.8261496225120111</v>
       </c>
       <c r="C6" t="n">
-        <v>0.718150479358624</v>
+        <v>0.838139974546402</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6844886753603293</v>
+        <v>0.8261496225120111</v>
       </c>
       <c r="E6" t="n">
-        <v>0.678974110704153</v>
+        <v>0.8265545525823867</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7059254175245938</v>
+        <v>0.8518874399450928</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7488661302646362</v>
+        <v>0.8579622526349604</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7059254175245938</v>
+        <v>0.8518874399450928</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7033312625658155</v>
+        <v>0.8518664635506795</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7037977579501258</v>
+        <v>0.8175245939144361</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7520611880317394</v>
+        <v>0.8279543546961212</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7037977579501258</v>
+        <v>0.8175245939144361</v>
       </c>
       <c r="M6" t="n">
-        <v>0.6995047456688194</v>
+        <v>0.8180653797168308</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7145504461221688</v>
+        <v>0.8411576298329901</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7359756673928738</v>
+        <v>0.8506178001618393</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7145504461221688</v>
+        <v>0.8411576298329901</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.7078176161253705</v>
+        <v>0.8407569444655187</v>
       </c>
       <c r="R6" t="n">
-        <v>0.7188515213909861</v>
+        <v>0.8497140242507436</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7455727442185192</v>
+        <v>0.8545892027115745</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7188515213909861</v>
+        <v>0.8497140242507436</v>
       </c>
       <c r="U6" t="n">
-        <v>0.712972901679728</v>
+        <v>0.8495344564060954</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7037977579501258</v>
+        <v>0.8561427590940289</v>
       </c>
       <c r="W6" t="n">
-        <v>0.7520611880317394</v>
+        <v>0.8624865978297163</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7037977579501258</v>
+        <v>0.8561427590940289</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6995047456688194</v>
+        <v>0.8566615758221836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>